<commit_message>
add vocabulary day 2
</commit_message>
<xml_diff>
--- a/developer_week_01.xlsx
+++ b/developer_week_01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIGUEL\Documents\workspace\EnglishDeveloper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9673EF2-2FDF-4D1F-8C6F-F7DA6C1472FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD77EE4C-B7F7-4C17-B4A5-F7C3ED0A5994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77C3AF13-D2D8-4AFD-961A-94EDE0097686}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="160">
   <si>
     <t>approach</t>
   </si>
@@ -129,9 +129,6 @@
     <t>single</t>
   </si>
   <si>
-    <t xml:space="preserve"> individuales</t>
-  </si>
-  <si>
     <t>attempt</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>even</t>
   </si>
   <si>
-    <t xml:space="preserve"> incluso</t>
-  </si>
-  <si>
     <t>improve</t>
   </si>
   <si>
@@ -156,21 +150,294 @@
     <t>towns</t>
   </si>
   <si>
-    <t xml:space="preserve"> pueblos</t>
+    <t>Word</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> translater</t>
+  </si>
+  <si>
+    <t>only</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> solo, único</t>
+  </si>
+  <si>
+    <t>within</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dentro</t>
+  </si>
+  <si>
+    <t>give</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dar</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> personal</t>
+  </si>
+  <si>
+    <t>curriculum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> plan de estudio</t>
+  </si>
+  <si>
+    <t>perform</t>
+  </si>
+  <si>
+    <t>complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> complejo</t>
+  </si>
+  <si>
+    <t>through</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a través</t>
+  </si>
+  <si>
+    <t>equip</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> equipar o proveer</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> equipo</t>
+  </si>
+  <si>
+    <t>Cipher</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cifrado</t>
+  </si>
+  <si>
+    <t>statements</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> declaraciones o enunciados o sentencias</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cualquier</t>
+  </si>
+  <si>
+    <t>keep</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> seguir o mantener</t>
+  </si>
+  <si>
+    <t>Whetting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> estimular o abrir el apetito</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> algunos</t>
+  </si>
+  <si>
+    <t>wish</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> desear</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> audio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /_a-'proch/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /meik/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'me-ni/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /moust/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'mei-jor/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /_a-vei'le-bol/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /seim/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'oun-li/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /ue-'den/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'ol-sou/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'poin-d_r/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /fer-d/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'su-re-bl/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'cas-to-mai-zebl/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'kau-vr/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'fi-ch_er/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'e-vri/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> individuales </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'sin-g_l/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> intentar </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /_a-'tempt/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /cam-pr_e-'jen-siv/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> incluso </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'i-ven/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /im-'pruv/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pueblos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /tauns/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /giv/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /staf/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /k_u-'r_i-c_u-l_on/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> realizar </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /pe-'form/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /k_om-'ples/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /fru/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /i-'kue/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /tim/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'sai-fer/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'stei-ments/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'eni/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /kip/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'ue-ding/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /sam/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /uich/</t>
+  </si>
+  <si>
+    <t>library</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> libreria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'lai-bre-ri/</t>
+  </si>
+  <si>
+    <t>party</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> parte o fiesta </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'pa-ri/</t>
+  </si>
+  <si>
+    <t>neighborhood</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vecindario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'nei-bor-ju/</t>
+  </si>
+  <si>
+    <t>enfoque</t>
   </si>
   <si>
     <t>hacer</t>
   </si>
   <si>
-    <t>muchas</t>
-  </si>
-  <si>
-    <t>mayoria</t>
+    <t>muchos</t>
+  </si>
+  <si>
+    <t>mayorira</t>
   </si>
   <si>
     <t>principal</t>
   </si>
   <si>
+    <t>disponible</t>
+  </si>
+  <si>
+    <t>mismo</t>
+  </si>
+  <si>
+    <t>algunos</t>
+  </si>
+  <si>
     <t>tambien</t>
   </si>
   <si>
@@ -180,6 +447,12 @@
     <t>terceros</t>
   </si>
   <si>
+    <t>adecuado</t>
+  </si>
+  <si>
+    <t>personalizable</t>
+  </si>
+  <si>
     <t>cubrir</t>
   </si>
   <si>
@@ -189,10 +462,13 @@
     <t>cada</t>
   </si>
   <si>
-    <t>individualmente</t>
-  </si>
-  <si>
-    <t>personalizable</t>
+    <t>individual</t>
+  </si>
+  <si>
+    <t>intentar</t>
+  </si>
+  <si>
+    <t>exhautivo</t>
   </si>
   <si>
     <t>incluso</t>
@@ -204,13 +480,40 @@
     <t>pueblos</t>
   </si>
   <si>
-    <t>exhautivo</t>
-  </si>
-  <si>
-    <t>mismo</t>
-  </si>
-  <si>
-    <t>intentar</t>
+    <t>dar</t>
+  </si>
+  <si>
+    <t>personal</t>
+  </si>
+  <si>
+    <t>complejo</t>
+  </si>
+  <si>
+    <t>a través</t>
+  </si>
+  <si>
+    <t>equipar</t>
+  </si>
+  <si>
+    <t>equipo</t>
+  </si>
+  <si>
+    <t>cifrado</t>
+  </si>
+  <si>
+    <t>setencias</t>
+  </si>
+  <si>
+    <t>desear</t>
+  </si>
+  <si>
+    <t>librería bibliotec</t>
+  </si>
+  <si>
+    <t>fiesta parte</t>
+  </si>
+  <si>
+    <t>vencindario</t>
   </si>
 </sst>
 </file>
@@ -562,235 +865,585 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E05C11-4F75-406C-839C-BDEFE0AE5243}">
-  <dimension ref="A2:D22"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" t="s">
         <v>45</v>
       </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>46</v>
       </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" t="s">
         <v>47</v>
       </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
+      <c r="D32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" t="s">
+        <v>158</v>
+      </c>
+      <c r="C41" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" t="s">
+        <v>159</v>
+      </c>
+      <c r="C42" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
words new in developer_weeek_01.txt
</commit_message>
<xml_diff>
--- a/developer_week_01.xlsx
+++ b/developer_week_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIGUEL\Documents\workspace\EnglishDeveloper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD77EE4C-B7F7-4C17-B4A5-F7C3ED0A5994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1EBA10-9A51-46D7-95C8-7B87D597DA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77C3AF13-D2D8-4AFD-961A-94EDE0097686}"/>
   </bookViews>
@@ -865,21 +865,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E05C11-4F75-406C-839C-BDEFE0AE5243}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -890,7 +891,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -904,7 +905,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -918,7 +919,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -931,8 +932,11 @@
       <c r="D4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -946,7 +950,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -959,8 +963,14 @@
       <c r="D6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -974,7 +984,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -988,7 +998,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -999,7 +1009,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1009,8 +1019,14 @@
       <c r="D10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1024,7 +1040,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1037,8 +1053,14 @@
       <c r="D12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1051,8 +1073,11 @@
       <c r="D13" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1065,8 +1090,14 @@
       <c r="D14" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1080,7 +1111,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1093,8 +1124,17 @@
       <c r="D16" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1107,8 +1147,14 @@
       <c r="D17" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1122,7 +1168,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1136,7 +1182,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1149,8 +1195,11 @@
       <c r="D20" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1164,7 +1213,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1178,7 +1227,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1192,7 +1241,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1206,7 +1255,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1219,8 +1268,14 @@
       <c r="D25" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1234,7 +1289,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1248,7 +1303,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1259,7 +1314,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1272,8 +1327,14 @@
       <c r="D29" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1287,7 +1348,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1301,7 +1362,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1315,7 +1376,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -1328,8 +1389,14 @@
       <c r="D33" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -1342,8 +1409,11 @@
       <c r="D34" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -1354,7 +1424,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -1365,7 +1435,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -1375,8 +1445,14 @@
       <c r="D37" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -1389,8 +1465,17 @@
       <c r="D38" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -1404,7 +1489,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -1418,7 +1503,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>120</v>
       </c>
@@ -1432,7 +1517,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>123</v>
       </c>

</xml_diff>

<commit_message>
add sound week 2
</commit_message>
<xml_diff>
--- a/developer_week_01.xlsx
+++ b/developer_week_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\C\Users\Ryzen\Documents\workspace\EnglishDeveloper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIGUEL\Documents\workspace\EnglishDeveloper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DB1D04-EC9B-41D2-9C4D-4D199419990B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC3020B-9D14-45E0-A3E7-CA27FA2794B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77C3AF13-D2D8-4AFD-961A-94EDE0097686}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{77C3AF13-D2D8-4AFD-961A-94EDE0097686}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -868,7 +868,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modelo en prisma avanzado
</commit_message>
<xml_diff>
--- a/developer_week_01.xlsx
+++ b/developer_week_01.xlsx
@@ -905,7 +905,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -916,8 +916,8 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add .dev and estructura_tablas.xls
</commit_message>
<xml_diff>
--- a/developer_week_01.xlsx
+++ b/developer_week_01.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\workspace\EnglishDeveloper\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C07CB4-C115-4262-BEFA-B1722446B6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -567,7 +564,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -905,19 +902,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,15 +922,15 @@
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="4" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -944,7 +941,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -957,11 +954,11 @@
       <c r="D2" t="s">
         <v>74</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -974,11 +971,11 @@
       <c r="D3" t="s">
         <v>75</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -991,14 +988,14 @@
       <c r="D4" t="s">
         <v>76</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1011,11 +1008,11 @@
       <c r="D5" t="s">
         <v>77</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1028,17 +1025,17 @@
       <c r="D6" t="s">
         <v>78</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1051,11 +1048,11 @@
       <c r="D7" t="s">
         <v>79</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1068,11 +1065,11 @@
       <c r="D8" t="s">
         <v>80</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1082,11 +1079,11 @@
       <c r="D9" t="s">
         <v>81</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1096,17 +1093,17 @@
       <c r="D10" t="s">
         <v>82</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1119,11 +1116,11 @@
       <c r="D11" t="s">
         <v>83</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1136,17 +1133,17 @@
       <c r="D12" t="s">
         <v>84</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
       <c r="F12">
         <v>1</v>
       </c>
-      <c r="I12" t="s">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1159,14 +1156,14 @@
       <c r="D13" t="s">
         <v>85</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1179,17 +1176,17 @@
       <c r="D14" t="s">
         <v>86</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="I14" t="s">
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1202,11 +1199,11 @@
       <c r="D15" t="s">
         <v>87</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1219,20 +1216,20 @@
       <c r="D16" t="s">
         <v>88</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="I16" t="s">
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1245,17 +1242,17 @@
       <c r="D17" t="s">
         <v>89</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
       <c r="F17">
         <v>1</v>
       </c>
-      <c r="I17" t="s">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1268,11 +1265,11 @@
       <c r="D18" t="s">
         <v>90</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1285,11 +1282,11 @@
       <c r="D19" t="s">
         <v>92</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1302,14 +1299,14 @@
       <c r="D20" t="s">
         <v>94</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1322,11 +1319,11 @@
       <c r="D21" t="s">
         <v>95</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1339,11 +1336,11 @@
       <c r="D22" t="s">
         <v>97</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1356,11 +1353,11 @@
       <c r="D23" t="s">
         <v>98</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1373,11 +1370,11 @@
       <c r="D24" t="s">
         <v>100</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1390,17 +1387,17 @@
       <c r="D25" t="s">
         <v>101</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1413,11 +1410,11 @@
       <c r="D26" t="s">
         <v>102</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1430,11 +1427,11 @@
       <c r="D27" t="s">
         <v>103</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1444,11 +1441,11 @@
       <c r="D28" t="s">
         <v>105</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1461,17 +1458,17 @@
       <c r="D29" t="s">
         <v>106</v>
       </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
       <c r="F29">
         <v>1</v>
       </c>
-      <c r="I29" t="s">
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1484,11 +1481,11 @@
       <c r="D30" t="s">
         <v>107</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1501,11 +1498,11 @@
       <c r="D31" t="s">
         <v>108</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1518,11 +1515,11 @@
       <c r="D32" t="s">
         <v>109</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -1535,17 +1532,17 @@
       <c r="D33" t="s">
         <v>110</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
       <c r="F33">
         <v>1</v>
       </c>
-      <c r="I33" t="s">
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -1558,14 +1555,14 @@
       <c r="D34" t="s">
         <v>111</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -1575,11 +1572,11 @@
       <c r="D35" t="s">
         <v>112</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -1589,11 +1586,11 @@
       <c r="D36" t="s">
         <v>113</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -1603,17 +1600,17 @@
       <c r="D37" t="s">
         <v>114</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
       <c r="F37">
         <v>1</v>
       </c>
-      <c r="I37" t="s">
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -1626,20 +1623,20 @@
       <c r="D38" t="s">
         <v>115</v>
       </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
       <c r="F38">
         <v>1</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="I38" t="s">
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -1652,11 +1649,11 @@
       <c r="D39" t="s">
         <v>116</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -1669,11 +1666,11 @@
       <c r="D40" t="s">
         <v>119</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>120</v>
       </c>
@@ -1686,11 +1683,11 @@
       <c r="D41" t="s">
         <v>122</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -1703,7 +1700,7 @@
       <c r="D42" t="s">
         <v>125</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>176</v>
       </c>
     </row>

</xml_diff>